<commit_message>
falta probar en la máquina virtual 091122 0504
</commit_message>
<xml_diff>
--- a/Cuentas recaudadoras/09.11.2022/CUENTAS DE CAJA IVSA.xlsx
+++ b/Cuentas recaudadoras/09.11.2022/CUENTAS DE CAJA IVSA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unipe-my.sharepoint.com/personal/20131022b_uni_pe/Documents/Venado/Cris/Traslado de tesoreria B5/Cuentas recaudadoras/09.11.2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_AA1A3038017B923EE464A49649B12E3E0DB9658F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40C086B9-5F44-4847-BE30-6B6562708FB2}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_AA1A3038017B923EE464A49649B12E3E0DB9658F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C1AED5B-4522-4624-963C-9623620F56D0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>CAJAS RECAUDADORAS A NIVEL NACIONAL</t>
   </si>
@@ -43,19 +43,22 @@
     <t>CAJA GENERAL M/N - RECAUDADORA</t>
   </si>
   <si>
-    <t>ENVIO DE RECAUDACION DIARIA</t>
-  </si>
-  <si>
     <t>ETV M.N</t>
   </si>
   <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA AGENCIA TARIJEÑITA</t>
-  </si>
-  <si>
-    <t>MCSC 1329</t>
-  </si>
-  <si>
-    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL COCHABAMBA</t>
+    <t>ENVIO DE RECAUDACION L-M-V</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG HONDURAS CBBA</t>
+  </si>
+  <si>
+    <t>BISA 0031</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA AG CALAMA CBBA</t>
+  </si>
+  <si>
+    <t>CAJA GENERAL M/N - RECAUDADORA CENTRAL SUCRE</t>
   </si>
   <si>
     <t>*NOTA: 1) LAS AGENCIAS MUY RARA VEZ RECIBEN DOLARES, GENERALMENTE ELMOVIMIENTO DIARIO SOLAMENTE ES EN DISTRIBUIDORA</t>
@@ -602,10 +605,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -907,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,25 +955,51 @@
       <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="37"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="39"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7">
+        <v>101010112</v>
+      </c>
+      <c r="D4" s="46">
+        <v>101044022</v>
+      </c>
+      <c r="E4" s="47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="9">
+        <v>101010113</v>
+      </c>
+      <c r="D5" s="42">
+        <v>101044022</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="39"/>
+      <c r="A6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="13">
+        <v>101010114</v>
+      </c>
+      <c r="D6" s="36">
+        <v>101020101</v>
+      </c>
+      <c r="E6" s="37" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14"/>
@@ -1034,57 +1059,19 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20"/>
-      <c r="B15" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="9">
-        <v>101010110</v>
-      </c>
-      <c r="D15" s="40">
-        <v>101041002</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>10</v>
-      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="41"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="13">
-        <v>101010111</v>
-      </c>
-      <c r="D16" s="36">
-        <v>101020101</v>
-      </c>
-      <c r="E16" s="37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="47"/>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="11"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
-    </row>
+      <c r="A16" s="21"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="37"/>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
@@ -1346,22 +1333,22 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="28" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1378,6 +1365,6 @@
     <mergeCell ref="D38:D40"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.38" bottom="0.27" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293"/>
 </worksheet>
 </file>
</xml_diff>